<commit_message>
Fin des erreurs restantes
</commit_message>
<xml_diff>
--- a/Documentation/Erreurs_restantes_EGS.xlsx
+++ b/Documentation/Erreurs_restantes_EGS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Description</t>
   </si>
@@ -42,6 +42,15 @@
   </si>
   <si>
     <t xml:space="preserve">Implémenter la ou les fonctionnalités permettant d'afficher l'heure sur l'horloge 60 LED </t>
+  </si>
+  <si>
+    <t>Améliorer l'algorithme pour rendre ces "mauvais clignotements" non visibles</t>
+  </si>
+  <si>
+    <t>Sur l'affichage 7 segments, durant le mode d'affichage de la température / heure / taux de CO2 en alternance, au moment de l'affichage de l'heure, l'affichage des secondes peut commencer par des clignotements plus rapides que les secondes reçues par la RTC</t>
+  </si>
+  <si>
+    <t>Les quelques premiers clignotements des secondes peuvent parfois être trop rapide par rapport aux secondes reçues par la RTC</t>
   </si>
 </sst>
 </file>
@@ -76,102 +85,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -189,71 +108,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -539,180 +407,186 @@
   <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" customWidth="1"/>
     <col min="4" max="4" width="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8">
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:8">
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:8" ht="36.75" customHeight="1">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="2:8" ht="75" customHeight="1">
-      <c r="B5" s="4" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:8" ht="60.75" customHeight="1">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="2:8" ht="71.25" customHeight="1" thickBot="1">
-      <c r="B6" s="11"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="2:8" ht="143.25" customHeight="1">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="2:8" ht="46.5" customHeight="1">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="2:8" ht="101.25" customHeight="1">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:8" ht="101.25" customHeight="1">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="2:8" ht="27" customHeight="1">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="2:8" ht="37.5" customHeight="1">
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="5:8">
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="5:8">
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="5:8" ht="150.75" customHeight="1">
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
     </row>
     <row r="20" spans="5:8" ht="51" customHeight="1"/>
   </sheetData>

</xml_diff>

<commit_message>
Fin de la documentation
</commit_message>
<xml_diff>
--- a/Documentation/Erreurs_restantes_EGS.xlsx
+++ b/Documentation/Erreurs_restantes_EGS.xlsx
@@ -35,15 +35,6 @@
     <t>Actions envisagées ou possibles</t>
   </si>
   <si>
-    <t>Le produit n'affiche pas l'heure sur l'horloge 60 LED</t>
-  </si>
-  <si>
-    <t>Il n'y a aucun moyen s'avoir l'heure en regardant l'horloge 60 LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implémenter la ou les fonctionnalités permettant d'afficher l'heure sur l'horloge 60 LED </t>
-  </si>
-  <si>
     <t>Améliorer l'algorithme pour rendre ces "mauvais clignotements" non visibles</t>
   </si>
   <si>
@@ -51,6 +42,15 @@
   </si>
   <si>
     <t>Les quelques premiers clignotements des secondes peuvent parfois être trop rapide par rapport aux secondes reçues par la RTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Il n’y a aucune indication indiquant que le capteur a besoin d’un certain temps avant d’afficher des valeurs correctes.</t>
+  </si>
+  <si>
+    <t>Le capteur du taux de CO2 (SGP30) a besoin de plusieurs secondes avant d’afficher la valeur correcte, il affichera durant ces 15 secondes « 400 » en permanence.</t>
+  </si>
+  <si>
+    <t>Implémenter une indication durant les 15 premières secondes indiquant que le capteur est en chargement</t>
   </si>
 </sst>
 </file>
@@ -406,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -459,15 +459,15 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:8" ht="60.75" customHeight="1">
+    <row r="5" spans="2:8" ht="129" customHeight="1">
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -476,13 +476,13 @@
     </row>
     <row r="6" spans="2:8" ht="143.25" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -517,7 +517,6 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="2:8" ht="101.25" customHeight="1">
-      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>

</xml_diff>